<commit_message>
added one txt file
</commit_message>
<xml_diff>
--- a/data/uws/SO289_UWS_continuous_file_list.xlsx
+++ b/data/uws/SO289_UWS_continuous_file_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ldelaigue\Documents\GitHub\SO289_cruise_processing\data\uws\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA26277-A865-45C8-BA24-F04BF9365EA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0957A2A6-D897-452B-8D40-E89D3DF77134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="710" windowWidth="14400" windowHeight="7360" xr2:uid="{AFFA04B0-61ED-42A2-921A-E115E7B57E02}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{AFFA04B0-61ED-42A2-921A-E115E7B57E02}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>sample</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>2022-03-24_003629_SO289_part_2</t>
+  </si>
+  <si>
+    <t>2022-02-24_221145_SO289</t>
   </si>
 </sst>
 </file>
@@ -570,7 +573,7 @@
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -590,7 +593,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -947,11 +953,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24354337-39CE-416A-A127-42BEC72437C4}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1004,7 +1010,7 @@
         <v>12</v>
       </c>
       <c r="D3" s="5"/>
-      <c r="E3" s="5">
+      <c r="E3" s="7">
         <v>2</v>
       </c>
     </row>
@@ -1019,7 +1025,7 @@
         <v>13</v>
       </c>
       <c r="D4" s="5"/>
-      <c r="E4" s="5">
+      <c r="E4" s="7">
         <v>2</v>
       </c>
     </row>
@@ -1033,7 +1039,7 @@
       <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="7">
         <v>2</v>
       </c>
     </row>
@@ -1047,7 +1053,21 @@
       <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="9">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="7">
         <v>2</v>
       </c>
     </row>

</xml_diff>